<commit_message>
1.2.2012: sua tiep bao cao chuong danh gia
</commit_message>
<xml_diff>
--- a/report/Final/ThongKeDuLieuThuThap.xlsx
+++ b/report/Final/ThongKeDuLieuThuThap.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="90" windowWidth="17235" windowHeight="9015" activeTab="5"/>
+    <workbookView xWindow="360" yWindow="90" windowWidth="17235" windowHeight="9015" tabRatio="728" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="Period_of_day" sheetId="1" r:id="rId1"/>
@@ -13,13 +13,14 @@
     <sheet name="budget" sheetId="4" r:id="rId4"/>
     <sheet name="companion" sheetId="5" r:id="rId5"/>
     <sheet name="weather" sheetId="6" r:id="rId6"/>
+    <sheet name="place" sheetId="7" r:id="rId7"/>
   </sheets>
   <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="50">
   <si>
     <t>period_of_day</t>
   </si>
@@ -27,15 +28,6 @@
     <t>Num</t>
   </si>
   <si>
-    <t>Morning</t>
-  </si>
-  <si>
-    <t>Night</t>
-  </si>
-  <si>
-    <t>Afternoon</t>
-  </si>
-  <si>
     <t>period_of_week</t>
   </si>
   <si>
@@ -48,61 +40,136 @@
     <t>season</t>
   </si>
   <si>
-    <t>Summer</t>
-  </si>
-  <si>
-    <t>Autumn</t>
-  </si>
-  <si>
-    <t>Spring</t>
-  </si>
-  <si>
-    <t>Winter</t>
-  </si>
-  <si>
     <t>budget</t>
   </si>
   <si>
-    <t>Budget traveler</t>
-  </si>
-  <si>
-    <t>High spender</t>
-  </si>
-  <si>
-    <t>Price for quality</t>
-  </si>
-  <si>
     <t>companion</t>
   </si>
   <si>
-    <t>Alone</t>
-  </si>
-  <si>
-    <t>Children</t>
-  </si>
-  <si>
-    <t>Family</t>
-  </si>
-  <si>
-    <t>Friends/Collegues</t>
-  </si>
-  <si>
-    <t>Girlfriend/Boyfriend</t>
-  </si>
-  <si>
     <t>weather</t>
   </si>
   <si>
-    <t>Clear sky</t>
-  </si>
-  <si>
-    <t>Cloudy</t>
-  </si>
-  <si>
-    <t>Rainy</t>
-  </si>
-  <si>
-    <t>Sunny</t>
+    <t>name</t>
+  </si>
+  <si>
+    <t>num</t>
+  </si>
+  <si>
+    <t>An Đông</t>
+  </si>
+  <si>
+    <t>Bến Thành</t>
+  </si>
+  <si>
+    <t>Bình Quới</t>
+  </si>
+  <si>
+    <t>Chợ Lớn</t>
+  </si>
+  <si>
+    <t>Nhà Thờ Chợ Quán</t>
+  </si>
+  <si>
+    <t>Bảo Tàng chứng tích chiến tranh</t>
+  </si>
+  <si>
+    <t>Đầm Sen nước</t>
+  </si>
+  <si>
+    <t>Diamon Plaza</t>
+  </si>
+  <si>
+    <t>Dinh Độc Lập</t>
+  </si>
+  <si>
+    <t>Nhà Thờ Đức Bà</t>
+  </si>
+  <si>
+    <t>Galaxy Cinema</t>
+  </si>
+  <si>
+    <t>Bảo Tàng HCM</t>
+  </si>
+  <si>
+    <t>Megastar Cinema</t>
+  </si>
+  <si>
+    <t>Nhà Hàng Món Huế</t>
+  </si>
+  <si>
+    <t>Phở 24h</t>
+  </si>
+  <si>
+    <t>Rex Hotel</t>
+  </si>
+  <si>
+    <t>Văn Thánh</t>
+  </si>
+  <si>
+    <t>Vĩnh Nghiêm</t>
+  </si>
+  <si>
+    <t>Winsord Plaza</t>
+  </si>
+  <si>
+    <t>Xá Lơi</t>
+  </si>
+  <si>
+    <t>Một mình</t>
+  </si>
+  <si>
+    <t>Trẻ em</t>
+  </si>
+  <si>
+    <t>Gia đình</t>
+  </si>
+  <si>
+    <t>Bạn bè/ đồng nghiệp</t>
+  </si>
+  <si>
+    <t>Người yêu</t>
+  </si>
+  <si>
+    <t>Trong xanh</t>
+  </si>
+  <si>
+    <t>Âm u, nhiều mây</t>
+  </si>
+  <si>
+    <t>Mưa</t>
+  </si>
+  <si>
+    <t>Nắng</t>
+  </si>
+  <si>
+    <t>Hè</t>
+  </si>
+  <si>
+    <t>Thu</t>
+  </si>
+  <si>
+    <t>Xuân</t>
+  </si>
+  <si>
+    <t>Đông</t>
+  </si>
+  <si>
+    <t>Sáng</t>
+  </si>
+  <si>
+    <t>Tối</t>
+  </si>
+  <si>
+    <t>Trưa, chiều</t>
+  </si>
+  <si>
+    <t>Đảm bảo cho chất lượng</t>
+  </si>
+  <si>
+    <t>Chi tiêu tiết kiệm</t>
+  </si>
+  <si>
+    <t>Chi tiêu sang trọng</t>
   </si>
 </sst>
 </file>
@@ -152,6 +219,676 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="110"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="10"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:pieChart>
+        <c:varyColors val="1"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:dLbls>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="0"/>
+            <c:showCatName val="1"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="1"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="1"/>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>Period_of_day!$A$2:$A$4</c:f>
+              <c:strCache>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>Sáng</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Tối</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Trưa, chiều</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Period_of_day!$B$2:$B$4</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>384</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>264</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>140</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="1"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="1"/>
+          <c:showBubbleSize val="0"/>
+          <c:showLeaderLines val="1"/>
+        </c:dLbls>
+        <c:firstSliceAng val="0"/>
+      </c:pieChart>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="110"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="10"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="1"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:pieChart>
+        <c:varyColors val="1"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:dLbls>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="0"/>
+            <c:showCatName val="1"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="1"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="1"/>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>Season!$A$2:$A$5</c:f>
+              <c:strCache>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>Hè</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Thu</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Xuân</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Đông</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Season!$B$2:$B$5</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>28</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>23</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>668</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>69</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="1"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="1"/>
+          <c:showBubbleSize val="0"/>
+          <c:showLeaderLines val="1"/>
+        </c:dLbls>
+        <c:firstSliceAng val="0"/>
+      </c:pieChart>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="110"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="10"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:pieChart>
+        <c:varyColors val="1"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:dLbls>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="0"/>
+            <c:showCatName val="1"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="1"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="1"/>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>budget!$A$2:$A$4</c:f>
+              <c:strCache>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>Chi tiêu tiết kiệm</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Chi tiêu sang trọng</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Đảm bảo cho chất lượng</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>budget!$B$2:$B$4</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>465</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>114</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>209</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="1"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="1"/>
+          <c:showBubbleSize val="0"/>
+          <c:showLeaderLines val="1"/>
+        </c:dLbls>
+        <c:firstSliceAng val="0"/>
+      </c:pieChart>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="110"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="10"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:pieChart>
+        <c:varyColors val="1"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:dLbls>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="0"/>
+            <c:showCatName val="1"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="1"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="1"/>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>companion!$A$2:$A$6</c:f>
+              <c:strCache>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>Một mình</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Trẻ em</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Gia đình</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Bạn bè/ đồng nghiệp</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Người yêu</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>companion!$B$2:$B$6</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>177</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>22</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>134</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>318</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>137</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="1"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="1"/>
+          <c:showBubbleSize val="0"/>
+          <c:showLeaderLines val="1"/>
+        </c:dLbls>
+        <c:firstSliceAng val="0"/>
+      </c:pieChart>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="110"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="10"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:pieChart>
+        <c:varyColors val="1"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:dLbls>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="0"/>
+            <c:showCatName val="1"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="1"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="1"/>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>weather!$A$2:$A$5</c:f>
+              <c:strCache>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>Trong xanh</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Âm u, nhiều mây</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Mưa</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Nắng</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>weather!$B$2:$B$5</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>301</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>44</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>35</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>408</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="1"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="1"/>
+          <c:showBubbleSize val="0"/>
+          <c:showLeaderLines val="1"/>
+        </c:dLbls>
+        <c:firstSliceAng val="0"/>
+      </c:pieChart>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>271462</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>128587</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>576262</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>14287</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>100012</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>176212</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>404812</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>61912</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>195262</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>128587</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>500062</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>14287</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>519112</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>128587</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>214312</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>14287</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing5.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>595312</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>128587</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>290512</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>14287</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -443,8 +1180,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+    <sheetView topLeftCell="D10" zoomScale="220" zoomScaleNormal="220" workbookViewId="0">
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -462,7 +1199,7 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>2</v>
+        <v>44</v>
       </c>
       <c r="B2">
         <v>384</v>
@@ -470,7 +1207,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>3</v>
+        <v>45</v>
       </c>
       <c r="B3">
         <v>264</v>
@@ -478,7 +1215,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>4</v>
+        <v>46</v>
       </c>
       <c r="B4">
         <v>140</v>
@@ -486,6 +1223,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -504,7 +1242,7 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>
@@ -512,7 +1250,7 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="B2">
         <v>365</v>
@@ -520,7 +1258,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="B3">
         <v>423</v>
@@ -535,8 +1273,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+    <sheetView topLeftCell="E4" zoomScale="200" zoomScaleNormal="200" workbookViewId="0">
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -546,7 +1284,7 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>
@@ -554,7 +1292,7 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>9</v>
+        <v>40</v>
       </c>
       <c r="B2">
         <v>28</v>
@@ -562,7 +1300,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>10</v>
+        <v>41</v>
       </c>
       <c r="B3">
         <v>23</v>
@@ -570,7 +1308,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>11</v>
+        <v>42</v>
       </c>
       <c r="B4">
         <v>668</v>
@@ -578,7 +1316,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>12</v>
+        <v>43</v>
       </c>
       <c r="B5">
         <v>69</v>
@@ -586,6 +1324,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -593,8 +1332,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+    <sheetView topLeftCell="E10" zoomScale="220" zoomScaleNormal="220" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -604,7 +1343,7 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>13</v>
+        <v>6</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>
@@ -612,7 +1351,7 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>14</v>
+        <v>48</v>
       </c>
       <c r="B2">
         <v>465</v>
@@ -620,7 +1359,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>15</v>
+        <v>49</v>
       </c>
       <c r="B3">
         <v>114</v>
@@ -628,7 +1367,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>16</v>
+        <v>47</v>
       </c>
       <c r="B4">
         <v>209</v>
@@ -636,6 +1375,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -643,8 +1383,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G29" sqref="G29"/>
+    <sheetView topLeftCell="E10" zoomScale="220" zoomScaleNormal="220" workbookViewId="0">
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -654,7 +1394,7 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>17</v>
+        <v>7</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>
@@ -662,7 +1402,7 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>18</v>
+        <v>31</v>
       </c>
       <c r="B2">
         <v>177</v>
@@ -670,7 +1410,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>19</v>
+        <v>32</v>
       </c>
       <c r="B3">
         <v>22</v>
@@ -678,7 +1418,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>20</v>
+        <v>33</v>
       </c>
       <c r="B4">
         <v>134</v>
@@ -686,7 +1426,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>21</v>
+        <v>34</v>
       </c>
       <c r="B5">
         <v>318</v>
@@ -694,7 +1434,7 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>22</v>
+        <v>35</v>
       </c>
       <c r="B6">
         <v>137</v>
@@ -702,6 +1442,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -709,15 +1450,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+    <sheetView tabSelected="1" topLeftCell="E10" zoomScale="200" zoomScaleNormal="200" workbookViewId="0">
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>23</v>
+        <v>8</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>
@@ -725,7 +1466,7 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>24</v>
+        <v>36</v>
       </c>
       <c r="B2">
         <v>301</v>
@@ -733,7 +1474,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>25</v>
+        <v>37</v>
       </c>
       <c r="B3">
         <v>44</v>
@@ -741,7 +1482,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>26</v>
+        <v>38</v>
       </c>
       <c r="B4">
         <v>35</v>
@@ -749,10 +1490,197 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>27</v>
+        <v>39</v>
       </c>
       <c r="B5">
         <v>408</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B21"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D25" sqref="D25"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="17.85546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B2">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B3">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>13</v>
+      </c>
+      <c r="B4">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>14</v>
+      </c>
+      <c r="B5">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>15</v>
+      </c>
+      <c r="B6">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>16</v>
+      </c>
+      <c r="B7">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>17</v>
+      </c>
+      <c r="B8">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>18</v>
+      </c>
+      <c r="B9">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>19</v>
+      </c>
+      <c r="B10">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>20</v>
+      </c>
+      <c r="B11">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>21</v>
+      </c>
+      <c r="B12">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>22</v>
+      </c>
+      <c r="B13">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>23</v>
+      </c>
+      <c r="B14">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>24</v>
+      </c>
+      <c r="B15">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>25</v>
+      </c>
+      <c r="B16">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>26</v>
+      </c>
+      <c r="B17">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>27</v>
+      </c>
+      <c r="B18">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>28</v>
+      </c>
+      <c r="B19">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>29</v>
+      </c>
+      <c r="B20">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>30</v>
+      </c>
+      <c r="B21">
+        <v>16</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
2.2.2012: bo sung bao cao, ve hinh slide
</commit_message>
<xml_diff>
--- a/report/Final/ThongKeDuLieuThuThap.xlsx
+++ b/report/Final/ThongKeDuLieuThuThap.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="90" windowWidth="17235" windowHeight="9015" tabRatio="728" activeTab="5"/>
+    <workbookView xWindow="360" yWindow="90" windowWidth="17235" windowHeight="9015" tabRatio="728" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="Period_of_day" sheetId="1" r:id="rId1"/>
@@ -55,66 +55,18 @@
     <t>num</t>
   </si>
   <si>
-    <t>An Đông</t>
-  </si>
-  <si>
-    <t>Bến Thành</t>
-  </si>
-  <si>
-    <t>Bình Quới</t>
-  </si>
-  <si>
-    <t>Chợ Lớn</t>
-  </si>
-  <si>
-    <t>Nhà Thờ Chợ Quán</t>
-  </si>
-  <si>
-    <t>Bảo Tàng chứng tích chiến tranh</t>
-  </si>
-  <si>
-    <t>Đầm Sen nước</t>
-  </si>
-  <si>
-    <t>Diamon Plaza</t>
-  </si>
-  <si>
-    <t>Dinh Độc Lập</t>
-  </si>
-  <si>
-    <t>Nhà Thờ Đức Bà</t>
-  </si>
-  <si>
     <t>Galaxy Cinema</t>
   </si>
   <si>
-    <t>Bảo Tàng HCM</t>
-  </si>
-  <si>
     <t>Megastar Cinema</t>
   </si>
   <si>
-    <t>Nhà Hàng Món Huế</t>
-  </si>
-  <si>
     <t>Phở 24h</t>
   </si>
   <si>
     <t>Rex Hotel</t>
   </si>
   <si>
-    <t>Văn Thánh</t>
-  </si>
-  <si>
-    <t>Vĩnh Nghiêm</t>
-  </si>
-  <si>
-    <t>Winsord Plaza</t>
-  </si>
-  <si>
-    <t>Xá Lơi</t>
-  </si>
-  <si>
     <t>Một mình</t>
   </si>
   <si>
@@ -170,6 +122,54 @@
   </si>
   <si>
     <t>Chi tiêu sang trọng</t>
+  </si>
+  <si>
+    <t>An Đông market</t>
+  </si>
+  <si>
+    <t>Bến Thành market</t>
+  </si>
+  <si>
+    <t>Bình Quới resort</t>
+  </si>
+  <si>
+    <t>Chợ Lớn market (Bình Tây market)</t>
+  </si>
+  <si>
+    <t>Chợ Quán church</t>
+  </si>
+  <si>
+    <t>Chứng Tích Chiến Tranh museum (War Remnants Museum)</t>
+  </si>
+  <si>
+    <t>Đầm Sen Water Park</t>
+  </si>
+  <si>
+    <t>Diamond Plaza</t>
+  </si>
+  <si>
+    <t>Dinh Độc Lập (Reunification Palace)</t>
+  </si>
+  <si>
+    <t>Đức Bà church (Saigon Notre-Dame Bassilica)</t>
+  </si>
+  <si>
+    <t>Ho Chi Minh Museum</t>
+  </si>
+  <si>
+    <t>Món Huế restaurant</t>
+  </si>
+  <si>
+    <t>Văn Thánh  resort</t>
+  </si>
+  <si>
+    <t>Vĩnh Nghiêm pagoda</t>
+  </si>
+  <si>
+    <t>Windsor Plaza Hotel</t>
+  </si>
+  <si>
+    <t>Xá Lơi pagoda</t>
   </si>
 </sst>
 </file>
@@ -472,13 +472,13 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>465</c:v>
+                  <c:v>415</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>114</c:v>
+                  <c:v>110</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>209</c:v>
+                  <c:v>203</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -573,19 +573,19 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>177</c:v>
+                  <c:v>127</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>22</c:v>
+                  <c:v>21</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>134</c:v>
+                  <c:v>132</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>318</c:v>
+                  <c:v>315</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>137</c:v>
+                  <c:v>133</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -677,16 +677,16 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>301</c:v>
+                  <c:v>295</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>44</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>35</c:v>
+                  <c:v>34</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>408</c:v>
+                  <c:v>355</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -861,15 +861,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>595312</xdr:colOff>
+      <xdr:colOff>595311</xdr:colOff>
       <xdr:row>6</xdr:row>
-      <xdr:rowOff>128587</xdr:rowOff>
+      <xdr:rowOff>128586</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>13</xdr:col>
-      <xdr:colOff>290512</xdr:colOff>
-      <xdr:row>21</xdr:row>
-      <xdr:rowOff>14287</xdr:rowOff>
+      <xdr:colOff>587374</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>134937</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1180,7 +1180,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView topLeftCell="D10" zoomScale="220" zoomScaleNormal="220" workbookViewId="0">
+    <sheetView topLeftCell="A6" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
       <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
@@ -1199,7 +1199,7 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>44</v>
+        <v>28</v>
       </c>
       <c r="B2">
         <v>384</v>
@@ -1207,7 +1207,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>45</v>
+        <v>29</v>
       </c>
       <c r="B3">
         <v>264</v>
@@ -1215,7 +1215,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>46</v>
+        <v>30</v>
       </c>
       <c r="B4">
         <v>140</v>
@@ -1292,7 +1292,7 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>40</v>
+        <v>24</v>
       </c>
       <c r="B2">
         <v>28</v>
@@ -1300,7 +1300,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>41</v>
+        <v>25</v>
       </c>
       <c r="B3">
         <v>23</v>
@@ -1308,7 +1308,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>42</v>
+        <v>26</v>
       </c>
       <c r="B4">
         <v>668</v>
@@ -1316,7 +1316,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>43</v>
+        <v>27</v>
       </c>
       <c r="B5">
         <v>69</v>
@@ -1330,10 +1330,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B4"/>
+  <dimension ref="A1:B6"/>
   <sheetViews>
-    <sheetView topLeftCell="E10" zoomScale="220" zoomScaleNormal="220" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1351,26 +1351,32 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>48</v>
+        <v>32</v>
       </c>
       <c r="B2">
-        <v>465</v>
+        <v>415</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>49</v>
+        <v>33</v>
       </c>
       <c r="B3">
-        <v>114</v>
+        <v>110</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>47</v>
+        <v>31</v>
       </c>
       <c r="B4">
-        <v>209</v>
+        <v>203</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B6">
+        <f>SUM(B2:B4)</f>
+        <v>728</v>
       </c>
     </row>
   </sheetData>
@@ -1381,10 +1387,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B6"/>
+  <dimension ref="A1:B8"/>
   <sheetViews>
-    <sheetView topLeftCell="E10" zoomScale="220" zoomScaleNormal="220" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1402,42 +1408,48 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>31</v>
+        <v>15</v>
       </c>
       <c r="B2">
-        <v>177</v>
+        <v>127</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>32</v>
+        <v>16</v>
       </c>
       <c r="B3">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>33</v>
+        <v>17</v>
       </c>
       <c r="B4">
-        <v>134</v>
+        <v>132</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>34</v>
+        <v>18</v>
       </c>
       <c r="B5">
-        <v>318</v>
+        <v>315</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>35</v>
+        <v>19</v>
       </c>
       <c r="B6">
-        <v>137</v>
+        <v>133</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B8">
+        <f>SUM(B2:B6)</f>
+        <v>728</v>
       </c>
     </row>
   </sheetData>
@@ -1448,10 +1460,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B5"/>
+  <dimension ref="A1:B7"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E10" zoomScale="200" zoomScaleNormal="200" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+    <sheetView topLeftCell="A7" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="M25" sqref="M25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1466,15 +1478,15 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>36</v>
+        <v>20</v>
       </c>
       <c r="B2">
-        <v>301</v>
+        <v>295</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>37</v>
+        <v>21</v>
       </c>
       <c r="B3">
         <v>44</v>
@@ -1482,18 +1494,24 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>38</v>
+        <v>22</v>
       </c>
       <c r="B4">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>39</v>
+        <v>23</v>
       </c>
       <c r="B5">
-        <v>408</v>
+        <v>355</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B7">
+        <f>SUM(B2:B5)</f>
+        <v>728</v>
       </c>
     </row>
   </sheetData>
@@ -1504,15 +1522,15 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B21"/>
+  <dimension ref="A1:B24"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D25" sqref="D25"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B25" sqref="B25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="17.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="54" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
@@ -1525,39 +1543,39 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>11</v>
+        <v>34</v>
       </c>
       <c r="B2">
-        <v>54</v>
+        <v>43</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>12</v>
+        <v>35</v>
       </c>
       <c r="B3">
-        <v>64</v>
+        <v>60</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>13</v>
+        <v>36</v>
       </c>
       <c r="B4">
-        <v>53</v>
+        <v>49</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>14</v>
+        <v>37</v>
       </c>
       <c r="B5">
-        <v>26</v>
+        <v>24</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>15</v>
+        <v>38</v>
       </c>
       <c r="B6">
         <v>5</v>
@@ -1565,122 +1583,128 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>16</v>
+        <v>39</v>
       </c>
       <c r="B7">
-        <v>39</v>
+        <v>35</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>17</v>
+        <v>40</v>
       </c>
       <c r="B8">
-        <v>81</v>
+        <v>78</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>18</v>
+        <v>41</v>
       </c>
       <c r="B9">
-        <v>45</v>
+        <v>43</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>19</v>
+        <v>42</v>
       </c>
       <c r="B10">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>20</v>
+        <v>43</v>
       </c>
       <c r="B11">
-        <v>63</v>
+        <v>59</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>21</v>
+        <v>11</v>
       </c>
       <c r="B12">
-        <v>53</v>
+        <v>50</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>22</v>
+        <v>44</v>
       </c>
       <c r="B13">
-        <v>24</v>
+        <v>19</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>23</v>
+        <v>12</v>
       </c>
       <c r="B14">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>24</v>
+        <v>45</v>
       </c>
       <c r="B15">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>25</v>
+        <v>13</v>
       </c>
       <c r="B16">
-        <v>52</v>
+        <v>49</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>26</v>
+        <v>14</v>
       </c>
       <c r="B17">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>27</v>
+        <v>46</v>
       </c>
       <c r="B18">
-        <v>36</v>
+        <v>32</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>28</v>
+        <v>47</v>
       </c>
       <c r="B19">
-        <v>24</v>
+        <v>20</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>29</v>
+        <v>48</v>
       </c>
       <c r="B20">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>30</v>
+        <v>49</v>
       </c>
       <c r="B21">
-        <v>16</v>
+        <v>15</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B24">
+        <f>SUM(B2:B21)</f>
+        <v>728</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
4.2.2012: slide + file thong ke
</commit_message>
<xml_diff>
--- a/report/Final/ThongKeDuLieuThuThap.xlsx
+++ b/report/Final/ThongKeDuLieuThuThap.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="90" windowWidth="17235" windowHeight="9015" tabRatio="728" activeTab="6"/>
+    <workbookView xWindow="360" yWindow="90" windowWidth="17235" windowHeight="9015" tabRatio="728" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="Period_of_day" sheetId="1" r:id="rId1"/>
@@ -280,13 +280,13 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>384</c:v>
+                  <c:v>393</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>264</c:v>
+                  <c:v>284</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>140</c:v>
+                  <c:v>143</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -374,16 +374,16 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>28</c:v>
+                  <c:v>30</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>23</c:v>
+                  <c:v>27</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>668</c:v>
+                  <c:v>692</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>69</c:v>
+                  <c:v>71</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -440,6 +440,21 @@
           <c:idx val="0"/>
           <c:order val="0"/>
           <c:dLbls>
+            <c:dLbl>
+              <c:idx val="1"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="0.14849190726159231"/>
+                  <c:y val="-0.10751130067074949"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="1"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="1"/>
+              <c:showBubbleSize val="0"/>
+            </c:dLbl>
             <c:showLegendKey val="0"/>
             <c:showVal val="0"/>
             <c:showCatName val="1"/>
@@ -472,13 +487,13 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>415</c:v>
+                  <c:v>487</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>110</c:v>
+                  <c:v>115</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>203</c:v>
+                  <c:v>218</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -573,19 +588,19 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>127</c:v>
+                  <c:v>192</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>21</c:v>
+                  <c:v>26</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>132</c:v>
+                  <c:v>139</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>315</c:v>
+                  <c:v>324</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>133</c:v>
+                  <c:v>139</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -642,6 +657,21 @@
           <c:idx val="0"/>
           <c:order val="0"/>
           <c:dLbls>
+            <c:dLbl>
+              <c:idx val="2"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-1.8499311887485735E-2"/>
+                  <c:y val="-9.3558336942938126E-3"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="1"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="1"/>
+              <c:showBubbleSize val="0"/>
+            </c:dLbl>
             <c:showLegendKey val="0"/>
             <c:showVal val="0"/>
             <c:showCatName val="1"/>
@@ -677,16 +707,16 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>295</c:v>
+                  <c:v>309</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>44</c:v>
+                  <c:v>47</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>34</c:v>
+                  <c:v>36</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>355</c:v>
+                  <c:v>428</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1178,10 +1208,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B4"/>
+  <dimension ref="A1:B6"/>
   <sheetViews>
-    <sheetView topLeftCell="A6" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+    <sheetView topLeftCell="E10" zoomScale="200" zoomScaleNormal="200" workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1202,7 +1232,7 @@
         <v>28</v>
       </c>
       <c r="B2">
-        <v>384</v>
+        <v>393</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
@@ -1210,7 +1240,7 @@
         <v>29</v>
       </c>
       <c r="B3">
-        <v>264</v>
+        <v>284</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
@@ -1218,7 +1248,13 @@
         <v>30</v>
       </c>
       <c r="B4">
-        <v>140</v>
+        <v>143</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B6">
+        <f>SUM(B2:B4)</f>
+        <v>820</v>
       </c>
     </row>
   </sheetData>
@@ -1229,10 +1265,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B3"/>
+  <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H12" sqref="H12"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1253,7 +1289,7 @@
         <v>3</v>
       </c>
       <c r="B2">
-        <v>365</v>
+        <v>370</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
@@ -1261,7 +1297,13 @@
         <v>4</v>
       </c>
       <c r="B3">
-        <v>423</v>
+        <v>450</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B5">
+        <f>SUM(B2:B3)</f>
+        <v>820</v>
       </c>
     </row>
   </sheetData>
@@ -1271,10 +1313,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B5"/>
+  <dimension ref="A1:B7"/>
   <sheetViews>
-    <sheetView topLeftCell="E4" zoomScale="200" zoomScaleNormal="200" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+    <sheetView topLeftCell="C3" zoomScale="180" zoomScaleNormal="180" workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1295,7 +1337,7 @@
         <v>24</v>
       </c>
       <c r="B2">
-        <v>28</v>
+        <v>30</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
@@ -1303,7 +1345,7 @@
         <v>25</v>
       </c>
       <c r="B3">
-        <v>23</v>
+        <v>27</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
@@ -1311,7 +1353,7 @@
         <v>26</v>
       </c>
       <c r="B4">
-        <v>668</v>
+        <v>692</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
@@ -1319,7 +1361,13 @@
         <v>27</v>
       </c>
       <c r="B5">
-        <v>69</v>
+        <v>71</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B7">
+        <f>SUM(B2:B5)</f>
+        <v>820</v>
       </c>
     </row>
   </sheetData>
@@ -1332,8 +1380,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B6"/>
   <sheetViews>
-    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+    <sheetView topLeftCell="D10" zoomScale="220" zoomScaleNormal="220" workbookViewId="0">
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1354,7 +1402,7 @@
         <v>32</v>
       </c>
       <c r="B2">
-        <v>415</v>
+        <v>487</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
@@ -1362,7 +1410,7 @@
         <v>33</v>
       </c>
       <c r="B3">
-        <v>110</v>
+        <v>115</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
@@ -1370,13 +1418,13 @@
         <v>31</v>
       </c>
       <c r="B4">
-        <v>203</v>
+        <v>218</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B6">
         <f>SUM(B2:B4)</f>
-        <v>728</v>
+        <v>820</v>
       </c>
     </row>
   </sheetData>
@@ -1389,8 +1437,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B8"/>
   <sheetViews>
-    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+    <sheetView topLeftCell="F10" zoomScale="220" zoomScaleNormal="220" workbookViewId="0">
+      <selection activeCell="M15" sqref="M15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1411,7 +1459,7 @@
         <v>15</v>
       </c>
       <c r="B2">
-        <v>127</v>
+        <v>192</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
@@ -1419,7 +1467,7 @@
         <v>16</v>
       </c>
       <c r="B3">
-        <v>21</v>
+        <v>26</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
@@ -1427,7 +1475,7 @@
         <v>17</v>
       </c>
       <c r="B4">
-        <v>132</v>
+        <v>139</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
@@ -1435,7 +1483,7 @@
         <v>18</v>
       </c>
       <c r="B5">
-        <v>315</v>
+        <v>324</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
@@ -1443,13 +1491,13 @@
         <v>19</v>
       </c>
       <c r="B6">
-        <v>133</v>
+        <v>139</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B8">
         <f>SUM(B2:B6)</f>
-        <v>728</v>
+        <v>820</v>
       </c>
     </row>
   </sheetData>
@@ -1462,8 +1510,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B7"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="M25" sqref="M25"/>
+    <sheetView tabSelected="1" topLeftCell="H10" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1481,7 +1529,7 @@
         <v>20</v>
       </c>
       <c r="B2">
-        <v>295</v>
+        <v>309</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
@@ -1489,7 +1537,7 @@
         <v>21</v>
       </c>
       <c r="B3">
-        <v>44</v>
+        <v>47</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
@@ -1497,7 +1545,7 @@
         <v>22</v>
       </c>
       <c r="B4">
-        <v>34</v>
+        <v>36</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
@@ -1505,13 +1553,13 @@
         <v>23</v>
       </c>
       <c r="B5">
-        <v>355</v>
+        <v>428</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B7">
         <f>SUM(B2:B5)</f>
-        <v>728</v>
+        <v>820</v>
       </c>
     </row>
   </sheetData>
@@ -1524,7 +1572,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B25" sqref="B25"/>
     </sheetView>
   </sheetViews>

</xml_diff>